<commit_message>
Updates of Master Data-Set
</commit_message>
<xml_diff>
--- a/WHO-DATA-SETS/ExcelDataSets/20200121-sitrep-1-2019-ncov.xlsx
+++ b/WHO-DATA-SETS/ExcelDataSets/20200121-sitrep-1-2019-ncov.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gunsl_000\Desktop\COVID-19 By Country\COVID-19-By-Country\WHO-DATA-SETS\ExcelDataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827D2347-F121-4509-A051-97678A9A3A69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C269C4F-6F6E-4731-8D5A-230F35A9549F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="3675" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,7 +225,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +242,12 @@
         <fgColor rgb="FFDBE4F0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -317,41 +323,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="6" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="7" shrinkToFit="1"/>
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="6" shrinkToFit="1"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,7 +700,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -705,13 +711,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -719,75 +725,75 @@
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="8">
         <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="12"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30">
       <c r="A4" s="12"/>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" s="12"/>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15">
       <c r="A6" s="12"/>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15">
       <c r="A7" s="12"/>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9">
+      <c r="B9" s="6"/>
+      <c r="C9" s="4">
         <v>282</v>
       </c>
     </row>
@@ -796,5 +802,6 @@
     <mergeCell ref="A2:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>